<commit_message>
Website content update with qmd file names corrected
</commit_message>
<xml_diff>
--- a/content/context/data/SArichnessupdated2025Aug6.xlsx
+++ b/content/context/data/SArichnessupdated2025Aug6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anisha\ProjectCollab\NBA2023-\BookletContent_biodiversityProfile\FinalQuarto\quarto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anisha\ProjectCollab\NBA2023-\BookletContent_biodiversityProfile\biodivprofLnkAboutP\about_webpages\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16C2187-30E8-451A-8823-9DA19EFB0C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640A0301-38CE-400E-AC95-17C08CD0548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3276" yWindow="2304" windowWidth="16548" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="0" windowWidth="9540" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,7 +638,7 @@
         <v>191</v>
       </c>
       <c r="D4" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -1017,15 +1017,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100475B28AE569E0040A3873194A0AB7E7F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a9da9b402df4a27855068f6b650c330">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4aa5c5e2-3ab7-4278-8876-7b89b552889a" xmlns:ns3="dc2f94d8-8575-44c3-a89c-8b8e78aa5398" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e45f7867d00cc9075482d5a3e2bafd5c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1271,6 +1262,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDB15CC-4EF8-45BB-9C84-DDE3C572CD65}">
   <ds:schemaRefs>
@@ -1284,14 +1284,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDC43A37-9E7E-4FD9-92C3-A71C0A3BA4F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06650D79-FC00-4D4D-8773-36BCB5D4A7D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1309,4 +1301,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDC43A37-9E7E-4FD9-92C3-A71C0A3BA4F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More or less working website
</commit_message>
<xml_diff>
--- a/content/context/data/SArichnessupdated2025Aug6.xlsx
+++ b/content/context/data/SArichnessupdated2025Aug6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anisha\ProjectCollab\NBA2023-\BookletContent_biodiversityProfile\biodivprofLnkAboutP\about_webpages\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640A0301-38CE-400E-AC95-17C08CD0548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C29106-B673-411B-861A-9D2DDC604D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="0" windowWidth="9540" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$9:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$8:$C$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Mammals</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Seaweed</t>
-  </si>
-  <si>
-    <t>Coral (hard and soft)</t>
   </si>
   <si>
     <t>Dung beetles</t>
@@ -562,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{708E5E81-9F99-4083-96F5-56774C04344B}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,13 +580,13 @@
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
@@ -616,106 +613,110 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>12961</v>
+        <v>1261</v>
       </c>
       <c r="C3" s="3">
-        <v>95</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>191</v>
+      </c>
+      <c r="D3" s="3">
+        <v>13</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
-        <v>1261</v>
+        <v>16500</v>
       </c>
       <c r="C4" s="3">
-        <v>191</v>
+        <v>2072</v>
       </c>
       <c r="D4" s="3">
-        <v>13</v>
+        <v>261</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4700</v>
+      </c>
+      <c r="C5" s="3">
+        <v>700</v>
+      </c>
+      <c r="D5" s="3">
+        <v>120</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3">
-        <v>16500</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2072</v>
-      </c>
-      <c r="D5" s="3">
-        <v>261</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="B6" s="3">
-        <v>4700</v>
+        <v>14628</v>
       </c>
       <c r="C6" s="3">
-        <v>700</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>14628</v>
+        <v>8896</v>
       </c>
       <c r="C7" s="3">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="D7" s="3">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
-        <v>8896</v>
+        <v>380000</v>
       </c>
       <c r="C8" s="3">
-        <v>135</v>
+        <v>21279</v>
       </c>
       <c r="D8" s="3">
-        <v>75</v>
+        <v>13965</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>380000</v>
+        <v>11494</v>
       </c>
       <c r="C9" s="3">
-        <v>21279</v>
+        <v>872</v>
       </c>
       <c r="D9" s="3">
-        <v>13965</v>
+        <v>156</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -723,85 +724,85 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B10" s="3">
-        <v>11494</v>
+        <v>6703</v>
       </c>
       <c r="C10" s="3">
-        <v>872</v>
+        <v>339</v>
       </c>
       <c r="D10" s="3">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
-        <v>6703</v>
+        <v>6200</v>
       </c>
       <c r="C11" s="3">
-        <v>339</v>
+        <v>600</v>
       </c>
       <c r="D11" s="3">
-        <v>67</v>
+        <v>221</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3">
-        <v>6200</v>
+        <v>52347</v>
       </c>
       <c r="C12" s="3">
-        <v>600</v>
+        <v>2214</v>
       </c>
       <c r="D12" s="3">
-        <v>221</v>
+        <v>1302</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:13" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3">
-        <v>52347</v>
+        <v>12440</v>
       </c>
       <c r="C13" s="3">
-        <v>2214</v>
+        <v>407</v>
       </c>
       <c r="D13" s="3">
-        <v>1302</v>
+        <v>155</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
-        <v>12440</v>
+        <v>20500</v>
       </c>
       <c r="C14" s="3">
-        <v>407</v>
+        <v>1253</v>
       </c>
       <c r="D14" s="3">
-        <v>155</v>
+        <v>646</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -809,16 +810,16 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B15" s="3">
-        <v>20500</v>
+        <v>17500</v>
       </c>
       <c r="C15" s="3">
-        <v>1253</v>
+        <v>799</v>
       </c>
       <c r="D15" s="3">
-        <v>646</v>
+        <v>419</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -826,16 +827,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>17500</v>
+        <v>6223</v>
       </c>
       <c r="C16" s="3">
-        <v>799</v>
+        <v>164</v>
       </c>
       <c r="D16" s="3">
-        <v>419</v>
+        <v>30</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -843,34 +844,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3">
-        <v>6223</v>
+        <v>12514</v>
       </c>
       <c r="C17" s="3">
-        <v>164</v>
+        <v>564</v>
       </c>
       <c r="D17" s="3">
-        <v>30</v>
+        <v>178</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3">
-        <v>12514</v>
-      </c>
-      <c r="C18" s="3">
-        <v>564</v>
-      </c>
-      <c r="D18" s="3">
-        <v>178</v>
-      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -891,44 +880,42 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="C28" s="1"/>
+      <c r="A27" s="3"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -943,10 +930,10 @@
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
@@ -958,8 +945,10 @@
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G40" s="3"/>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
@@ -990,11 +979,6 @@
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1017,6 +1001,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100475B28AE569E0040A3873194A0AB7E7F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a9da9b402df4a27855068f6b650c330">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4aa5c5e2-3ab7-4278-8876-7b89b552889a" xmlns:ns3="dc2f94d8-8575-44c3-a89c-8b8e78aa5398" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e45f7867d00cc9075482d5a3e2bafd5c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1262,15 +1255,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EDB15CC-4EF8-45BB-9C84-DDE3C572CD65}">
   <ds:schemaRefs>
@@ -1284,6 +1268,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDC43A37-9E7E-4FD9-92C3-A71C0A3BA4F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06650D79-FC00-4D4D-8773-36BCB5D4A7D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1301,12 +1293,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDC43A37-9E7E-4FD9-92C3-A71C0A3BA4F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>